<commit_message>
Updated the python script name just to remove the white space making directory work easier
Explicitly added variable names to remove errors seen by FrancoisGLEYZON when compiling the script
This should create the base set of Transient variable names when transient variables are used

I also fixed the convective boundary conditions in the example transient file. I had them in fahrenheit instead of Kelvin

Signed-off-by: blackpressinc <blackpressinc@gmail.com>
</commit_message>
<xml_diff>
--- a/Example_Transient_Boundary_Conditions.xlsx
+++ b/Example_Transient_Boundary_Conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Transfer\Fraser Jones\1D Transient Toolbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black\Desktop\1D_Transient_Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205FE595-7001-4CDE-A66C-C73DC0DC95F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6308AAA-DE20-4131-A860-C44D583CC6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="3780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8250" yWindow="1215" windowWidth="20550" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,6 +154,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,7 +443,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +554,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="5">
-        <v>37.999999999999986</v>
+        <v>338</v>
       </c>
       <c r="E4" s="6">
         <v>0.8</v>
@@ -575,6 +578,7 @@
       <c r="K4" s="4">
         <v>0</v>
       </c>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -588,7 +592,7 @@
         <v>28.725930513988288</v>
       </c>
       <c r="D5" s="5">
-        <v>73.360492908262842</v>
+        <v>373.36049290826281</v>
       </c>
       <c r="E5" s="6">
         <v>0.8</v>
@@ -612,6 +616,7 @@
       <c r="K5" s="4">
         <v>0</v>
       </c>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -625,7 +630,7 @@
         <v>39.200441418281841</v>
       </c>
       <c r="D6" s="5">
-        <v>93.843971734870934</v>
+        <v>393.84397173487093</v>
       </c>
       <c r="E6" s="6">
         <v>0.8</v>
@@ -649,6 +654,7 @@
       <c r="K6" s="4">
         <v>0</v>
       </c>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -662,7 +668,7 @@
         <v>57.502139513922977</v>
       </c>
       <c r="D7" s="5">
-        <v>97.07268476914939</v>
+        <v>397.07268476914942</v>
       </c>
       <c r="E7" s="6">
         <v>0.8</v>
@@ -686,6 +692,7 @@
       <c r="K7" s="4">
         <v>0</v>
       </c>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -699,7 +706,7 @@
         <v>76.290168123076924</v>
       </c>
       <c r="D8" s="5">
-        <v>100.20388923076924</v>
+        <v>400.20388923076922</v>
       </c>
       <c r="E8" s="6">
         <v>0.8</v>
@@ -723,6 +730,7 @@
       <c r="K8" s="4">
         <v>0</v>
       </c>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -736,7 +744,7 @@
         <v>99.455171353846154</v>
       </c>
       <c r="D9" s="5">
-        <v>102.45751653846153</v>
+        <v>402.4575165384615</v>
       </c>
       <c r="E9" s="6">
         <v>0.8</v>
@@ -760,6 +768,7 @@
       <c r="K9" s="4">
         <v>0</v>
       </c>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -773,7 +782,7 @@
         <v>95.663509163636377</v>
       </c>
       <c r="D10" s="5">
-        <v>105.71975770909091</v>
+        <v>405.71975770909091</v>
       </c>
       <c r="E10" s="6">
         <v>0.8</v>
@@ -797,6 +806,7 @@
       <c r="K10" s="4">
         <v>0</v>
       </c>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -810,7 +820,7 @@
         <v>187.32752218490566</v>
       </c>
       <c r="D11" s="5">
-        <v>167.34845835471708</v>
+        <v>467.34845835471708</v>
       </c>
       <c r="E11" s="6">
         <v>0.8</v>
@@ -834,6 +844,7 @@
       <c r="K11" s="4">
         <v>0</v>
       </c>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -847,7 +858,7 @@
         <v>174.68591909917359</v>
       </c>
       <c r="D12" s="5">
-        <v>320.19989906280966</v>
+        <v>620.19989906280966</v>
       </c>
       <c r="E12" s="6">
         <v>0.8</v>
@@ -871,6 +882,7 @@
       <c r="K12" s="4">
         <v>0</v>
       </c>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -884,7 +896,7 @@
         <v>92.095159871287024</v>
       </c>
       <c r="D13" s="5">
-        <v>440.9040332079208</v>
+        <v>740.90403320792075</v>
       </c>
       <c r="E13" s="6">
         <v>0.8</v>
@@ -908,6 +920,7 @@
       <c r="K13" s="4">
         <v>0</v>
       </c>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -921,7 +934,7 @@
         <v>41.394672867441841</v>
       </c>
       <c r="D14" s="5">
-        <v>520.10071332558141</v>
+        <v>820.10071332558141</v>
       </c>
       <c r="E14" s="6">
         <v>0.8</v>
@@ -945,6 +958,7 @@
       <c r="K14" s="4">
         <v>0</v>
       </c>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -958,7 +972,7 @@
         <v>20.18870100909092</v>
       </c>
       <c r="D15" s="5">
-        <v>1007.742647181818</v>
+        <v>1307.742647181818</v>
       </c>
       <c r="E15" s="6">
         <v>0.8</v>
@@ -982,6 +996,7 @@
       <c r="K15" s="4">
         <v>0</v>
       </c>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -995,7 +1010,7 @@
         <v>12.139967556716421</v>
       </c>
       <c r="D16" s="5">
-        <v>2766.8760752238741</v>
+        <v>3066.8760752238741</v>
       </c>
       <c r="E16" s="6">
         <v>0.8</v>
@@ -1019,8 +1034,9 @@
       <c r="K16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -1032,7 +1048,7 @@
         <v>10.25745305645161</v>
       </c>
       <c r="D17" s="5">
-        <v>5056.5527475806448</v>
+        <v>5356.5527475806448</v>
       </c>
       <c r="E17" s="6">
         <v>0.8</v>
@@ -1056,8 +1072,9 @@
       <c r="K17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -1069,7 +1086,7 @@
         <v>11.242309196296297</v>
       </c>
       <c r="D18" s="5">
-        <v>5418.7685433333345</v>
+        <v>5718.7685433333345</v>
       </c>
       <c r="E18" s="6">
         <v>0.8</v>
@@ -1093,8 +1110,9 @@
       <c r="K18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>150</v>
@@ -1106,7 +1124,7 @@
         <v>13.069267113114755</v>
       </c>
       <c r="D19" s="5">
-        <v>6010.8523568852461</v>
+        <v>6310.8523568852461</v>
       </c>
       <c r="E19" s="6">
         <v>0.8</v>
@@ -1130,8 +1148,9 @@
       <c r="K19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -1143,7 +1162,7 @@
         <v>13.245141521739132</v>
       </c>
       <c r="D20" s="5">
-        <v>6175.8209899999993</v>
+        <v>6475.8209899999993</v>
       </c>
       <c r="E20" s="6">
         <v>0.8</v>
@@ -1167,8 +1186,9 @@
       <c r="K20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>170</v>
@@ -1180,7 +1200,7 @@
         <v>11.658877208480568</v>
       </c>
       <c r="D21" s="5">
-        <v>5592.6174734982305</v>
+        <v>5892.6174734982305</v>
       </c>
       <c r="E21" s="6">
         <v>0.8</v>
@@ -1204,8 +1224,9 @@
       <c r="K21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="1"/>
         <v>180</v>
@@ -1217,7 +1238,7 @@
         <v>9.3271017667844518</v>
       </c>
       <c r="D22" s="5">
-        <v>4494.0939787985844</v>
+        <v>4794.0939787985844</v>
       </c>
       <c r="E22" s="6">
         <v>0.8</v>
@@ -1241,8 +1262,9 @@
       <c r="K22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>190</v>
       </c>
@@ -1253,7 +1275,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="5">
-        <v>3000</v>
+        <v>3300</v>
       </c>
       <c r="E23" s="6">
         <v>0.8</v>
@@ -1277,6 +1299,7 @@
       <c r="K23" s="4">
         <v>0</v>
       </c>
+      <c r="L23" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>